<commit_message>
solucion salidas y otros cambios
</commit_message>
<xml_diff>
--- a/files/reports/parametros/reporte_concetrado_modulo_A.xlsx
+++ b/files/reports/parametros/reporte_concetrado_modulo_A.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Reporte Modulo A</t>
   </si>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Semana: </t>
   </si>
   <si>
-    <t>2019/04/12 al 2019/04/14</t>
+    <t>2020/02/01 al 2020/02/25</t>
   </si>
   <si>
     <t/>
@@ -59,6 +59,66 @@
   </si>
   <si>
     <t>pH</t>
+  </si>
+  <si>
+    <t>Promedios S-01 :</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>S-02</t>
+  </si>
+  <si>
+    <t>LUNES</t>
+  </si>
+  <si>
+    <t>30.20</t>
+  </si>
+  <si>
+    <t>34.20</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>5.50</t>
+  </si>
+  <si>
+    <t>180.00</t>
+  </si>
+  <si>
+    <t>120.00</t>
+  </si>
+  <si>
+    <t>22.00</t>
+  </si>
+  <si>
+    <t>7.90</t>
+  </si>
+  <si>
+    <t>Promedios S-02 :</t>
+  </si>
+  <si>
+    <t>Promedios del módulo:</t>
+  </si>
+  <si>
+    <t>12.88</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>23.50</t>
+  </si>
+  <si>
+    <t>7.40</t>
   </si>
 </sst>
 </file>
@@ -69,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -100,8 +160,18 @@
       <sz val="12"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+      <sz val="12"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +189,19 @@
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="848484"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="848484"/>
+        <bgColor rgb="000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -128,11 +209,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="#FFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="#FFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="#FFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#FFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -146,6 +242,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -608,9 +722,137 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="12">
+        <v>43885.29166666667</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A9:K9"/>
-  <mergeCells count="7">
+  <mergeCells count="10">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="F4:G4"/>
@@ -618,6 +860,9 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>